<commit_message>
added feature file for story ID_007
</commit_message>
<xml_diff>
--- a/deliverables/work/sprint_a/backlog.xlsx
+++ b/deliverables/work/sprint_a/backlog.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E206E362-8477-45E2-AF7B-4A7849605C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yixuan Qin\Desktop\ALLOCOR\deliverables\work\sprint_a\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D22B47-92BD-4DFB-9338-DC2DFD34D0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5895" yWindow="3780" windowWidth="21735" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint A" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Identifier</t>
   </si>
@@ -96,42 +101,51 @@
     <t>Delete user account</t>
   </si>
   <si>
+    <t>ID006</t>
+  </si>
+  <si>
+    <t>Reset user password</t>
+  </si>
+  <si>
+    <t>Implement in future sprint</t>
+  </si>
+  <si>
+    <t>Not Groomed</t>
+  </si>
+  <si>
+    <t>ID007</t>
+  </si>
+  <si>
+    <t>Update user details</t>
+  </si>
+  <si>
+    <t>ID008</t>
+  </si>
+  <si>
+    <t>Persist user sessions</t>
+  </si>
+  <si>
+    <t>Implement in next sprint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>ID005_delete_account.feature</t>
-  </si>
-  <si>
-    <t>ID006</t>
-  </si>
-  <si>
-    <t>Reset user password</t>
-  </si>
-  <si>
-    <t>Implement in future sprint</t>
-  </si>
-  <si>
-    <t>Not Groomed</t>
-  </si>
-  <si>
-    <t>ID007</t>
-  </si>
-  <si>
-    <t>Update user details</t>
-  </si>
-  <si>
-    <t>ID008</t>
-  </si>
-  <si>
-    <t>Persist user sessions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID007_update_user_details.feature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -139,7 +153,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -554,19 +575,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="35.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -617,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -634,7 +655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -651,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -665,55 +686,58 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>